<commit_message>
submit new AUDUSD model and minmax
</commit_message>
<xml_diff>
--- a/Predicciones/save_predictions_GBPAUD.xlsx
+++ b/Predicciones/save_predictions_GBPAUD.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK159"/>
+  <dimension ref="A1:AK160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14062,6 +14062,91 @@
         <v>71.74552007</v>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2025-06-16T00:15</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>GBPAUD</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>0.0004192503380775411</v>
+      </c>
+      <c r="E160" t="inlineStr"/>
+      <c r="F160" t="inlineStr"/>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="inlineStr"/>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" t="inlineStr"/>
+      <c r="K160" t="inlineStr"/>
+      <c r="L160" t="inlineStr"/>
+      <c r="M160" t="inlineStr"/>
+      <c r="N160" t="inlineStr"/>
+      <c r="O160" t="inlineStr"/>
+      <c r="P160" t="inlineStr"/>
+      <c r="Q160" t="inlineStr"/>
+      <c r="R160" t="inlineStr"/>
+      <c r="S160" t="inlineStr"/>
+      <c r="T160" t="inlineStr"/>
+      <c r="U160" t="inlineStr"/>
+      <c r="V160" t="n">
+        <v>2.08842</v>
+      </c>
+      <c r="W160" t="n">
+        <v>2.08766</v>
+      </c>
+      <c r="X160" t="n">
+        <v>2.08842</v>
+      </c>
+      <c r="Y160" t="n">
+        <v>2.08766</v>
+      </c>
+      <c r="Z160" t="n">
+        <v>104</v>
+      </c>
+      <c r="AA160" t="n">
+        <v>2.08842</v>
+      </c>
+      <c r="AB160" t="n">
+        <v>2.08774</v>
+      </c>
+      <c r="AC160" t="n">
+        <v>2.08842</v>
+      </c>
+      <c r="AD160" t="n">
+        <v>2.08774</v>
+      </c>
+      <c r="AE160" t="n">
+        <v>206</v>
+      </c>
+      <c r="AF160" t="n">
+        <v>16.58752366</v>
+      </c>
+      <c r="AG160" t="n">
+        <v>26.98794612</v>
+      </c>
+      <c r="AH160" t="n">
+        <v>10.93155894</v>
+      </c>
+      <c r="AI160" t="n">
+        <v>26.85330452</v>
+      </c>
+      <c r="AJ160" t="n">
+        <v>33.89830508</v>
+      </c>
+      <c r="AK160" t="n">
+        <v>44.53840033</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>